<commit_message>
tao nhanh moi va thu data dchs
</commit_message>
<xml_diff>
--- a/4-chuyen-json-file/output_1.xlsx
+++ b/4-chuyen-json-file/output_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52" count="52">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87" count="87">
   <x:si>
     <x:t>Url</x:t>
   </x:si>
@@ -100,10 +100,10 @@
     <x:t>SEO Description</x:t>
   </x:si>
   <x:si>
-    <x:t>Danh_mục</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Danh_mục_EN</x:t>
+    <x:t>Danh mục</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Danh mục EN</x:t>
   </x:si>
   <x:si>
     <x:t>Ảnh biến thể</x:t>
@@ -112,65 +112,29 @@
     <x:t>Không áp dụng khuyến mãi</x:t>
   </x:si>
   <x:si>
-    <x:t>slime-unicorn-collectible-slimy-33911-ye-bl---mu-vng--xanh-ngc---unicorn-trng</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Slime Unicorn Collectible Slimy 33911-YE-BL - Màu Vàng + Xanh Ngọc - Unicorn Trắng</x:t>
-  </x:si>
-  <x:si>
-    <x:t>- Thông tin chi tiết
-- Mã hàng
-- 8935247318781-mau2
-- Độ Tuổi
-- 5+
-- Tên Nhà Cung Cấp
-- Việt Tinh Anh
-- Năm XB
-- 2021
-- Thương Hiệu
-- Slimy
-- Xuất Xứ Thương Hiệu
-- Thương Hiệu Thụy Sĩ
-- Nơi Gia Công &amp; Sản Xuất
-- Trung Quốc
-- Màu sắc
-- Vàng - Xanh Ngọc
-- Chất liệu
-- Bột, Nước, Nhựa
-- Thông Số Kỹ Thuật
-- Không Dùng Pin
-- Thông Tin Cảnh Báo
-- Không thích hợp cho trẻ dưới 5 tuổi
-- Hướng Dẫn Sử Dụng
-- Dùng chơi bằng tay
-- Trọng lượng (gr)
-- 203
-- Kích Thước Bao Bì
-- 13 x 6 x 6 cm
-- Sản phẩm bán chạy nhất	Top 100 sản phẩm Slime - Chất Nhờn Ma Quái bán chạy của tháng
-- Giá sản phẩm trên Fabico
-- com đã bao gồm thuế theo luật hiện hành
-- Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,
-- Chính sách khuyến mãi trên Fabico
-- com không áp dụng cho Hệ thống Nhà sách Fabico trên toàn quốc
-- Slime Unicorn Collectible Slimy 33911-YE-BL
-- SLIMY là tên một thứ đồ chơi bắt nguồn từ nước ngoài lấy ý tưởng khởi nguồn từ một câu chuyện về những quái vật ma quái biết biến thành muôn hình vạn trạng để thoát khỏi sự truy đuổi của con người
-- Slimy là một dạng chất dẻo đặc biệt với đặc tính mềm dẻo của cao su nhưng lại mềm mại như nước, biến đổi theo hình dạng vật thể chứa nó
-- Đồ chơi Slimy chất nhờn ma quái chuẩn có thể chui lọt lỗ kim, có thể kéo sợi mảnh như tơ, biến đổi hình dạng bất ngờ và nhanh chóng do đó, người chơi phải hết sức nhanh nhẹn và linh hoạt trong cách chơi
-- Sản phẩm có màu tự nhiên, hương liệu dùng trong thực phẩm, đảm bảo an toàn khi chơi cùng, thành phần không độc hại hay gây kích ứng cho trẻ nhỏ cả khi tiếp xúc thường xuyên
-- Bộ sản phẩm không chỉ đơn giản là món đồ chơi cho trẻ nhỏ, thông qua việc tạo hình, bé sẽ phần nào tạo được nên tảng về nghệ thuật, cách phối màu, tạo hình cho sự vật
-- Trí tưởng tượng của trẻ nhỏ từ đó cũng có thể được kích thích trở nên rộng mở hơn, cho con trẻ định hình được khả năng của bản thân
-- Bộ sưu tập Slimy unicorn với 2 loại slime khác nhau trong cùng 1 hũ, chất slime mềm đàn hồi cực thích
-- 1 chú unicorn đi kèm cùng hũ Slimy
-- Hãy sưu tập trọn bộ ngay 12 nhân vật Unicorn cực dễ thương này nhé!
-- Thương hiệu đến từ Thụy Sĩ an toàn tuyệt đối cho da bé nhạy cảm
-- Xem thêm</x:t>
+    <x:t>bt-bi-05-mm-laris---thin-long-tl-095---mc-xanh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bút Bi 0.5 mm Laris - Thiên Long TL-095 - Mực Xanh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;table cellpadding="8" cellspacing="0" style="width: 100%; max-width: 600px; border-collapse: collapse;"&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Mã hàng&lt;/th&gt;&lt;td style="text-align: left;"&gt;8935001804079&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Tên Nhà Cung Cấp&lt;/th&gt;&lt;td style="text-align: left;"&gt;Thiên Long Hoàn Cầu&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Thương Hiệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Thiên Long&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Xuất Xứ Thương Hiệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Việt Nam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Nơi Gia Công &amp; Sản Xuất&lt;/th&gt;&lt;td style="text-align: left;"&gt;Việt Nam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Màu sắc&lt;/th&gt;&lt;td style="text-align: left;"&gt;Xanh Dương&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Màu Mực&lt;/th&gt;&lt;td style="text-align: left;"&gt;Đỏ&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Chất liệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Nhựa&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Trọng lượng (gr)&lt;/th&gt;&lt;td style="text-align: left;"&gt;20&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Kích Thước Bao Bì&lt;/th&gt;&lt;td style="text-align: left;"&gt;14 x 1 x 1 cm&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Sản phẩm hiển thị trong&lt;/th&gt;&lt;td style="text-align: left;"&gt;B2S - Lớp 6 - 2022&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;B2S - Lớp 7 - 2022&lt;/th&gt;&lt;td style="text-align: left;"&gt;B2S - Lớp 8 - 2022&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;B2S - Lớp 9 - 2022&lt;/th&gt;&lt;td style="text-align: left;"&gt;Ông Trùm Trường Học&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;BACK TO SCHOOL&lt;/th&gt;&lt;td style="text-align: left;"&gt;Sách Giáo Khoa - Tham Khảo Các Cấp&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Thiên Long Hoàn Cầu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Sản phẩm bán chạy nhất	Top 100 sản phẩm Bút Bi bán chạy của tháng&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Giá sản phẩm trên Fabico.vn đã bao gồm thuế theo luật hiện hành. Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,...&lt;/th&gt;&lt;td style="text-align: left;"&gt;Chính sách khuyến mãi trên Fabico.vn không áp dụng cho Hệ thống Nhà sách Fahasa trên toàn quốc&lt;/td&gt;&lt;/tr&gt;
+        &lt;tr&gt;
+            &lt;td colspan="2" style="text-align: left;"&gt;
+                Giá sản phẩm trên Fabico.vn đã bao gồm thuế theo luật hiện hành. Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,...&lt;br&gt;
+                Chính sách khuyến mãi trên Fabico.vn không áp dụng cho Hệ thống Nhà sách Fabico trên toàn quốc.
+            &lt;/td&gt;
+        &lt;/tr&gt;
+    &lt;/table&gt;
+Bút Bi 0.5 mm Laris - Thiên Long TL-095 có thiết kế đột phá với cơ cấu bấm sáng tạo: Ruột tự động bật lên khi cài giắt bút vào túi áo.
+Kiểu dáng hiện đại, phần tay cầm có đệm cao su mềm (grip) giúp cho cầm bút rất thoải mái.
+Viết rất trơn, êm, mực ra đều, liên tục, đầu bút dạng needle và màu mực: 0.5mm.</x:t>
   </x:si>
   <x:si>
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>Việt Tinh Anh</x:t>
+    <x:t>Thiên Long Hoàn Cầu</x:t>
   </x:si>
   <x:si>
     <x:t>Yes</x:t>
@@ -191,31 +155,167 @@
     <x:t>Tác giả</x:t>
   </x:si>
   <x:si>
+    <x:t>Tác Giả</x:t>
+  </x:si>
+  <x:si>
     <x:t>Haravan</x:t>
   </x:si>
   <x:si>
     <x:t>continue</x:t>
   </x:si>
   <x:si>
-    <x:t>8935247318781-mau2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cdn0.fahasa.com/media/catalog/product/i/m/image_237680.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Đồ chơi giáo dục</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935247318781-mau2-_5_.jpg</x:t>
+    <x:t>8935001804079</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/thumbnailframe/product_frame_ncc/frame_8935001804079-mau1-_3_.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BÚT - VIẾT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>but-viet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804079-mau1-_3_.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>no</x:t>
   </x:si>
   <x:si>
-    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935247318781-mau2-_6_.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935247318781-mau2-_3_.jpg</x:t>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086_7__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086-_4__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086-_3__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086_5__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086_6__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086_8__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086-_1__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804079-mau1-_1_.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804079_3.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804079-mau1-_4_.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001804086_9__1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bt-bi-pastel-pro-027-05-mm---thin-long-tl-105---mc-xanh-mu-thn-bt-giao-ngu-nhin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bút Bi Pastel Pro 027 0.5 mm - Thiên Long TL-105 - Mực Xanh (Màu Thân Bút Giao Ngẫu Nhiên)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;table cellpadding="8" cellspacing="0" style="width: 100%; max-width: 600px; border-collapse: collapse;"&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Mã hàng&lt;/th&gt;&lt;td style="text-align: left;"&gt;8935324002893&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Tên Nhà Cung Cấp&lt;/th&gt;&lt;td style="text-align: left;"&gt;Thiên Long Hoàn Cầu&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Thương Hiệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Thiên Long&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Xuất Xứ Thương Hiệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Việt Nam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Nơi Gia Công &amp; Sản Xuất&lt;/th&gt;&lt;td style="text-align: left;"&gt;Việt Nam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Màu sắc&lt;/th&gt;&lt;td style="text-align: left;"&gt;Nhiều màu&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Màu Mực&lt;/th&gt;&lt;td style="text-align: left;"&gt;Xanh&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Chất liệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Nhựa&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Trọng lượng (gr)&lt;/th&gt;&lt;td style="text-align: left;"&gt;15&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Kích Thước Bao Bì&lt;/th&gt;&lt;td style="text-align: left;"&gt;14 x 1 x 1 cm&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Sản phẩm bán chạy nhất&lt;/th&gt;&lt;td style="text-align: left;"&gt;Top 100 sản phẩm Bút Bi bán chạy của tháng&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Giá sản phẩm trên Fabico.vn đã bao gồm thuế theo luật hiện hành. Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,...&lt;/th&gt;&lt;td style="text-align: left;"&gt;Chính sách khuyến mãi trên Fabico.vn không áp dụng cho Hệ thống Nhà sách Fahasa trên toàn quốc&lt;/td&gt;&lt;/tr&gt;
+        &lt;tr&gt;
+            &lt;td colspan="2" style="text-align: left;"&gt;
+                Giá sản phẩm trên Fabico.vn đã bao gồm thuế theo luật hiện hành. Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,...&lt;br&gt;
+                Chính sách khuyến mãi trên Fabico.vn không áp dụng cho Hệ thống Nhà sách Fabico trên toàn quốc.
+            &lt;/td&gt;
+        &lt;/tr&gt;
+    &lt;/table&gt;
+Bút Bi Pastel Pro 027 0.5 mm - Thiên Long TL-105 - Mực Xanh
+- Thân bút màu pastel thời trang.
+- Mực êm trơn, đều, mượt, không chảy mực.
+- Lực kẹp giắt chắc chắn, có thể cài được sổ bìa dày 3 mm.
+- Cơ cấu bấm sáng tạo, tự thu ngòi khi cài bút vào tập - túi áo - sổ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8935324002893</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/thumbnailframe/product_frame_ncc/frame_8935324002893-0.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-0.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau2-_1__1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau3-_1__1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau4-_3__1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau2-_2.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau4-_1__1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau2-_3__1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935324002893-mau2-_4__1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bt-bi-05-mm-thin-long-tl-027---mc-xanh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bút Bi 0.5 mm Thiên Long TL-027 - Mực Xanh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;table cellpadding="8" cellspacing="0" style="width: 100%; max-width: 600px; border-collapse: collapse;"&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Mã hàng&lt;/th&gt;&lt;td style="text-align: left;"&gt;8935001800347&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Tên Nhà Cung Cấp&lt;/th&gt;&lt;td style="text-align: left;"&gt;Thiên Long Hoàn Cầu&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Thương Hiệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Thiên Long&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Xuất Xứ Thương Hiệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Việt Nam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Nơi Gia Công &amp; Sản Xuất&lt;/th&gt;&lt;td style="text-align: left;"&gt;Việt Nam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Màu sắc&lt;/th&gt;&lt;td style="text-align: left;"&gt;Xanh Dương&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Màu Mực&lt;/th&gt;&lt;td style="text-align: left;"&gt;Xanh&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Chất liệu&lt;/th&gt;&lt;td style="text-align: left;"&gt;Nhựa, Kim Loại&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Trọng lượng (gr)&lt;/th&gt;&lt;td style="text-align: left;"&gt;10&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Kích Thước Bao Bì&lt;/th&gt;&lt;td style="text-align: left;"&gt;14 x 0.7 x 0.7 cm&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Sản phẩm bán chạy nhất&lt;/th&gt;&lt;td style="text-align: left;"&gt;Top 100 sản phẩm Bút Bi bán chạy của tháng&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th style="text-align: left;"&gt;Giá sản phẩm trên Fabico.vn đã bao gồm thuế theo luật hiện hành. Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,...&lt;/th&gt;&lt;td style="text-align: left;"&gt;Chính sách khuyến mãi trên Fabico.vn không áp dụng cho Hệ thống Nhà sách Fahasa trên toàn quốc&lt;/td&gt;&lt;/tr&gt;
+        &lt;tr&gt;
+            &lt;td colspan="2" style="text-align: left;"&gt;
+                Giá sản phẩm trên Fabico.vn đã bao gồm thuế theo luật hiện hành. Bên cạnh đó, tuỳ vào loại sản phẩm, hình thức và địa chỉ giao hàng mà có thể phát sinh thêm chi phí khác như Phụ phí đóng gói, phí vận chuyển, phụ phí hàng cồng kềnh,...&lt;br&gt;
+                Chính sách khuyến mãi trên Fabico.vn không áp dụng cho Hệ thống Nhà sách Fabico trên toàn quốc.
+            &lt;/td&gt;
+        &lt;/tr&gt;
+    &lt;/table&gt;
+Bút Bi Thiên Long TL-027 - Mực Xanh
+Đây là một trong những cây bút đang được học sinh sử dụng nhiều nhất tại Việt Nam. Bút có thiết kế tối giản, nhưng tinh tế và ấn tượng. Toàn bộ thân bút làm từ nhựa trong, phối hợp hoàn hảo với màu ruột bút bên trong.
+Đặc điểm:
+- Đầu bi: 0.5mm, sản xuất tại Thụy Sĩ.
+- Bút bi dạng bấm cò.
+- Nơi tì ngón tay có tiết diện hình tam giác vừa vặn với tay cầm giúp giảm trơn tuột khi viết thường xuyên.
+- Mực đạt chuẩn: ASTM D-4236, ASTM F 963-91, EN71/3, TSCA.
+Lợi ích:
+- Đầu bi nhỏ cho nét chữ thanh mảnh.
+- Cơ chế bấm nằm gọn dưới giắt bút, giúp thuận tay khi sử dụng.
+- Thay ruột khi hết mực.
+Xem thêm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8935001800347</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/thumbnailframe/product_frame_ncc/frame_8935001800347_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001800347_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001800347-3.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001800347-2.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001800347-1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn0.fahasa.com/media/catalog/product/8/9/8935001800347-4.jpg</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -717,7 +817,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="N2" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
         <x:v>35</x:v>
@@ -726,19 +826,19 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="R2" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="T2" s="0" t="n">
-        <x:v>107100</x:v>
+        <x:v>9775</x:v>
       </x:c>
       <x:c r="U2" s="0" t="n">
-        <x:v>119000</x:v>
+        <x:v>11500</x:v>
       </x:c>
       <x:c r="V2" s="0" t="s">
         <x:v>37</x:v>
@@ -747,10 +847,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="X2" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="Y2" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="s">
         <x:v>35</x:v>
@@ -762,16 +862,16 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="AC2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="AD2" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="AE2" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AF2" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:32">
@@ -848,7 +948,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="Y3" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="Z3" s="0" t="s">
         <x:v>35</x:v>
@@ -946,7 +1046,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="Y4" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="Z4" s="0" t="s">
         <x:v>35</x:v>
@@ -1044,27 +1144,2477 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="Y5" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Z5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:32">
+      <x:c r="A6" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y6" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="Z6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:32">
+      <x:c r="A7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y7" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="Z7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:32">
+      <x:c r="A8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y8" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Z8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:32">
+      <x:c r="A9" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y9" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="Z9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:32">
+      <x:c r="A10" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y10" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Z10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:32">
+      <x:c r="A11" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y11" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="Z11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:32">
+      <x:c r="A12" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y12" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="Z12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF12" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:32">
+      <x:c r="A13" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y13" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="Z13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:32">
+      <x:c r="A14" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y14" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="Z14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:32">
+      <x:c r="A15" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I15" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K15" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="L15" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="M15" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="N15" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="O15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P15" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="Q15" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R15" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="S15" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="T15" s="0" t="n">
+        <x:v>5525</x:v>
+      </x:c>
+      <x:c r="U15" s="0" t="n">
+        <x:v>6500</x:v>
+      </x:c>
+      <x:c r="V15" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="W15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X15" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="Y15" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="Z15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA15" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="AB15" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="AC15" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AD15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE15" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AF15" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="Z5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="AA5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="AB5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="AC5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="AD5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="AE5" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="AF5" s="0" t="s">
+    </x:row>
+    <x:row r="16" spans="1:32">
+      <x:c r="A16" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y16" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="Z16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF16" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:32">
+      <x:c r="A17" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y17" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="Z17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:32">
+      <x:c r="A18" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y18" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Z18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF18" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:32">
+      <x:c r="A19" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y19" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="Z19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:32">
+      <x:c r="A20" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y20" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="Z20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF20" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:32">
+      <x:c r="A21" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y21" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="Z21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF21" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:32">
+      <x:c r="A22" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y22" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="Z22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:32">
+      <x:c r="A23" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y23" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Z23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF23" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:32">
+      <x:c r="A24" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y24" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF24" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:32">
+      <x:c r="A25" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G25" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="H25" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I25" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J25" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K25" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="L25" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="M25" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="N25" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="O25" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P25" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="Q25" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R25" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="S25" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="T25" s="0" t="n">
+        <x:v>5100</x:v>
+      </x:c>
+      <x:c r="U25" s="0" t="n">
+        <x:v>6000</x:v>
+      </x:c>
+      <x:c r="V25" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="W25" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X25" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="Y25" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="Z25" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA25" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="AB25" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="AC25" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AD25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE25" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="AF25" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:32">
+      <x:c r="A26" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y26" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="Z26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:32">
+      <x:c r="A27" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y27" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="Z27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF27" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:32">
+      <x:c r="A28" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y28" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="Z28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF28" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:32">
+      <x:c r="A29" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y29" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="Z29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF29" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:32">
+      <x:c r="A30" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="K30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="M30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="N30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="O30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="P30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Q30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="R30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="S30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="U30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="V30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="W30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="Y30" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="Z30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AA30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AB30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AC30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AD30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AE30" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AF30" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
     </x:row>

</xml_diff>